<commit_message>
something is broken so this branch is disconinued now
</commit_message>
<xml_diff>
--- a/Bestpractices.xlsx
+++ b/Bestpractices.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\Documents\GitHub\openBest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF5E95A-2BAB-4139-93C9-AA881234234C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6640DE6-1D34-44B8-BB92-DCE463B8A5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C7A31B53-E591-4299-A46F-3D8228156FE2}"/>
   </bookViews>
@@ -96,12 +96,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Written by</t>
-  </si>
-  <si>
-    <t>Reviewed by</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -178,6 +172,12 @@
   </si>
   <si>
     <t>Example Description</t>
+  </si>
+  <si>
+    <t>Written</t>
+  </si>
+  <si>
+    <t>Reviewed</t>
   </si>
 </sst>
 </file>
@@ -567,13 +567,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F728DF5-5A10-40A1-9B0E-54C243945F9E}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" customWidth="1"/>
     <col min="4" max="4" width="39.109375" customWidth="1"/>
     <col min="5" max="5" width="37.44140625" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
@@ -624,128 +624,128 @@
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="Q1" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
       </c>
       <c r="K2" s="5">
         <v>44451</v>
       </c>
       <c r="L2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N2" t="s">
         <v>0</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" t="s">
-        <v>37</v>
-      </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K3" s="5">
         <v>44481</v>
       </c>
       <c r="L3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N3" t="s">
         <v>0</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Continued, added functional best practice loading script
</commit_message>
<xml_diff>
--- a/Bestpractices.xlsx
+++ b/Bestpractices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\Documents\GitHub\openBest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6640DE6-1D34-44B8-BB92-DCE463B8A5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AD35AF-66E0-4729-96C0-B0F426FD4B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C7A31B53-E591-4299-A46F-3D8228156FE2}"/>
   </bookViews>
@@ -567,14 +567,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F728DF5-5A10-40A1-9B0E-54C243945F9E}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="39.109375" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" customWidth="1"/>
     <col min="5" max="5" width="37.44140625" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>

</xml_diff>

<commit_message>
Expanded table view, from here the tool is tailored towards the ECG
</commit_message>
<xml_diff>
--- a/Bestpractices.xlsx
+++ b/Bestpractices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\Documents\GitHub\openBest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AD35AF-66E0-4729-96C0-B0F426FD4B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CDE6FF-5E26-4E71-8A75-6BDCADFE3465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C7A31B53-E591-4299-A46F-3D8228156FE2}"/>
   </bookViews>
@@ -184,6 +184,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="dd\-mm\-yy;@"/>
+    <numFmt numFmtId="171" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -225,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
@@ -233,7 +237,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F728DF5-5A10-40A1-9B0E-54C243945F9E}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,7 +588,7 @@
     <col min="7" max="7" width="22" customWidth="1"/>
     <col min="8" max="8" width="25.33203125" customWidth="1"/>
     <col min="9" max="9" width="20.88671875" customWidth="1"/>
-    <col min="11" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.44140625" style="6" customWidth="1"/>
     <col min="12" max="12" width="16.33203125" customWidth="1"/>
     <col min="13" max="13" width="15.5546875" customWidth="1"/>
     <col min="14" max="14" width="15" customWidth="1"/>
@@ -622,7 +628,7 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
@@ -675,8 +681,8 @@
       <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="5">
-        <v>44451</v>
+      <c r="K2" s="7">
+        <v>44587</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -728,8 +734,8 @@
       <c r="J3" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="5">
-        <v>44481</v>
+      <c r="K3" s="7">
+        <v>44587</v>
       </c>
       <c r="L3" t="s">
         <v>31</v>
@@ -754,7 +760,6 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="K4" s="5"/>
       <c r="O4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
@@ -762,7 +767,6 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="K5" s="5"/>
       <c r="O5" s="1"/>
       <c r="Q5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Fixed table filter functionality
</commit_message>
<xml_diff>
--- a/Bestpractices.xlsx
+++ b/Bestpractices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\Documents\GitHub\openBest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CDE6FF-5E26-4E71-8A75-6BDCADFE3465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F9E2C0-8F20-44AD-BD8C-CFA2C98AA350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C7A31B53-E591-4299-A46F-3D8228156FE2}"/>
+    <workbookView xWindow="1344" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{C7A31B53-E591-4299-A46F-3D8228156FE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>Effort</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Reviewed</t>
+  </si>
+  <si>
+    <t>Prevention instead of aftercare</t>
   </si>
 </sst>
 </file>
@@ -185,8 +188,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="dd\-mm\-yy;@"/>
-    <numFmt numFmtId="171" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -237,9 +240,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F728DF5-5A10-40A1-9B0E-54C243945F9E}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,7 +670,7 @@
         <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
         <v>26</v>

</xml_diff>